<commit_message>
Correção da implementação e testes do método del
</commit_message>
<xml_diff>
--- a/CasoDeTesteMetodoDel.xlsx
+++ b/CasoDeTesteMetodoDel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Método de teste delTrueTest</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>Método de teste delListaVaziaTest</t>
-  </si>
-  <si>
-    <t>Método de teste delValorInexistenteTest</t>
   </si>
 </sst>
 </file>
@@ -147,7 +144,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -183,7 +180,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>4</v>
@@ -228,40 +225,9 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="n">
-        <v>-1</v>
-      </c>
-    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>